<commit_message>
Added test entry to setlist
</commit_message>
<xml_diff>
--- a/setlist.xlsx
+++ b/setlist.xlsx
@@ -19,16 +19,52 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original Interpret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cover Interpret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabs / Chords von</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American Pie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don McLean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G-Dur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tabs.ultimate-guitar.com/d/don_mclean/american_pie_ver2_crd.htm</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+  <fonts count="17">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -46,51 +82,99 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -191,25 +275,65 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -306,17 +430,60 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="61.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="https://tabs.ultimate-guitar.com/d/don_mclean/american_pie_ver2_crd.htm"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>